<commit_message>
style: restructuring of the repo
</commit_message>
<xml_diff>
--- a/not_loaded.xlsx
+++ b/not_loaded.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,270 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040629', 'EBCN2517914')</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>80</v>
+      </c>
+      <c r="C2" t="n">
+        <v>120</v>
+      </c>
+      <c r="D2" t="n">
+        <v>102</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040359', 'EBCN2517757')</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>80</v>
+      </c>
+      <c r="C3" t="n">
+        <v>120</v>
+      </c>
+      <c r="D3" t="n">
+        <v>71</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040609', 'EBCN2517913')</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>120</v>
+      </c>
+      <c r="C4" t="n">
+        <v>80</v>
+      </c>
+      <c r="D4" t="n">
+        <v>68</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040331', 'EBCN2517748')</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>78</v>
+      </c>
+      <c r="C5" t="n">
+        <v>64</v>
+      </c>
+      <c r="D5" t="n">
+        <v>108</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040313', 'EBCN2517556')</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>89</v>
+      </c>
+      <c r="C6" t="n">
+        <v>62</v>
+      </c>
+      <c r="D6" t="n">
+        <v>90</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040330', 'EBCN2517562')</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>61</v>
+      </c>
+      <c r="C7" t="n">
+        <v>77</v>
+      </c>
+      <c r="D7" t="n">
+        <v>102</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040108', 'EBCN2517554')</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>61</v>
+      </c>
+      <c r="C8" t="n">
+        <v>79</v>
+      </c>
+      <c r="D8" t="n">
+        <v>88</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040628', 'EBCN2517914')</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>120</v>
+      </c>
+      <c r="C9" t="n">
+        <v>80</v>
+      </c>
+      <c r="D9" t="n">
+        <v>39</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040604', 'EBCN2517897')</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>79</v>
+      </c>
+      <c r="C10" t="n">
+        <v>65</v>
+      </c>
+      <c r="D10" t="n">
+        <v>64</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040360', 'EBCN2517758')</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>80</v>
+      </c>
+      <c r="C11" t="n">
+        <v>64</v>
+      </c>
+      <c r="D11" t="n">
+        <v>51</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040317', 'EBCN2517744')</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>36</v>
+      </c>
+      <c r="C12" t="n">
+        <v>32</v>
+      </c>
+      <c r="D12" t="n">
+        <v>25</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>('SBCN25040358', 'EBCN2517756')</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>50</v>
+      </c>
+      <c r="C13" t="n">
+        <v>32</v>
+      </c>
+      <c r="D13" t="n">
+        <v>22</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>